<commit_message>
Updated the comparison chart
</commit_message>
<xml_diff>
--- a/Project/MPI_Comparison.xlsx
+++ b/Project/MPI_Comparison.xlsx
@@ -22,7 +22,7 @@
     <t>time</t>
   </si>
   <si>
-    <t>1E6 histories</t>
+    <t>1E5 histories</t>
   </si>
 </sst>
 </file>
@@ -177,11 +177,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="284932304"/>
-        <c:axId val="367332064"/>
+        <c:axId val="202919288"/>
+        <c:axId val="281377392"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="284932304"/>
+        <c:axId val="202919288"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -238,12 +238,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="367332064"/>
+        <c:crossAx val="281377392"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="367332064"/>
+        <c:axId val="281377392"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -300,7 +300,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="284932304"/>
+        <c:crossAx val="202919288"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1230,7 +1230,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P10" sqref="P10"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1274,6 +1274,9 @@
       <c r="B5">
         <v>24.13</v>
       </c>
+      <c r="C5">
+        <v>21.67</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -1281,6 +1284,9 @@
       </c>
       <c r="B6">
         <v>19.95</v>
+      </c>
+      <c r="C6">
+        <v>17.27</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Just moved the project proposal into the project folder
</commit_message>
<xml_diff>
--- a/Project/MPI_Comparison.xlsx
+++ b/Project/MPI_Comparison.xlsx
@@ -9,12 +9,12 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Nodes</t>
   </si>
@@ -24,18 +24,33 @@
   <si>
     <t>1E5 histories</t>
   </si>
+  <si>
+    <t>Jermey</t>
+  </si>
+  <si>
+    <t>Me</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -58,8 +73,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -128,9 +144,6 @@
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
-                <c:pt idx="0">
-                  <c:v>0</c:v>
-                </c:pt>
                 <c:pt idx="1">
                   <c:v>1</c:v>
                 </c:pt>
@@ -148,21 +161,24 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$6</c:f>
+              <c:f>Sheet1!$C$2:$C$6</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
                 <c:pt idx="1">
-                  <c:v>66.98</c:v>
+                  <c:v>60.15</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>34.380000000000003</c:v>
+                  <c:v>31.26</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.13</c:v>
+                  <c:v>21.67</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>19.95</c:v>
+                  <c:v>17.27</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -177,13 +193,15 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="202919288"/>
-        <c:axId val="281377392"/>
+        <c:axId val="286630456"/>
+        <c:axId val="206236440"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="202919288"/>
+        <c:axId val="286630456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="4"/>
+          <c:min val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -201,6 +219,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Number of Nodes</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -230,20 +307,20 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="281377392"/>
+        <c:crossAx val="206236440"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="281377392"/>
+        <c:axId val="206236440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -263,6 +340,65 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US">
+                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  </a:rPr>
+                  <a:t>Execution Time</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -292,15 +428,15 @@
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
+                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
+                <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="202919288"/>
+        <c:crossAx val="286630456"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -909,16 +1045,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
+      <xdr:col>5</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>90487</xdr:rowOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>14287</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
+      <xdr:col>12</xdr:col>
       <xdr:colOff>304800</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>166687</xdr:rowOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>90487</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1227,66 +1363,91 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="P14" sqref="P14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="16384" width="9.140625" style="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>0</v>
+      <c r="B2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3">
+      <c r="A3" s="1">
         <v>1</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="1">
         <v>66.98</v>
+      </c>
+      <c r="C3" s="1">
+        <v>60.15</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4">
+      <c r="A4" s="1">
         <v>2</v>
       </c>
-      <c r="B4">
+      <c r="B4" s="1">
         <v>34.380000000000003</v>
+      </c>
+      <c r="C4" s="1">
+        <v>31.26</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5">
+      <c r="A5" s="1">
         <v>3</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="1">
         <v>24.13</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>21.67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6">
+      <c r="A6" s="1">
         <v>4</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="1">
         <v>19.95</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="1">
         <v>17.27</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="1">
+        <f>B3/B6</f>
+        <v>3.3573934837092736</v>
+      </c>
+      <c r="C8" s="1">
+        <f>C3/C6</f>
+        <v>3.4829183555298204</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added papers for review
</commit_message>
<xml_diff>
--- a/Project/MPI_Comparison.xlsx
+++ b/Project/MPI_Comparison.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>Nodes</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>Original</t>
   </si>
 </sst>
 </file>
@@ -193,11 +196,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="286630456"/>
-        <c:axId val="206236440"/>
+        <c:axId val="211519568"/>
+        <c:axId val="303936952"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="286630456"/>
+        <c:axId val="211519568"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="4"/>
@@ -315,12 +318,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206236440"/>
+        <c:crossAx val="303936952"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206236440"/>
+        <c:axId val="303936952"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -436,7 +439,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="286630456"/>
+        <c:crossAx val="211519568"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1363,10 +1366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D8"/>
+  <dimension ref="A1:D10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1450,6 +1453,14 @@
         <v>3.4829183555298204</v>
       </c>
     </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="1">
+        <v>77.709999999999994</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>